<commit_message>
CVE ANALYSTICS Version 3
</commit_message>
<xml_diff>
--- a/Data/Component_Data.xlsx
+++ b/Data/Component_Data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1362"/>
+  <dimension ref="A1:B1376"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16473,6 +16473,174 @@
         </is>
       </c>
     </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>ActiproSoftware.SyntaxEditor.Addons.DotNet.Wpf.dll</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Charts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>ActiproSoftware.SyntaxEditor.Addons.JavaScript.Wpf.dll</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Charts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>ActiproSoftware.SyntaxEditor.Addons.Xml.Wpf.dll</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Charts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>ActiproSoftware.SyntaxEditor.Wpf.dll</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Charts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>ActiproSoftware.Text.Addons.DotNet.Roslyn.Wpf.dll</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Charts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>ActiproSoftware.Text.Addons.DotNet.Wpf.dll</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Charts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>ActiproSoftware.Text.Addons.JavaScript.Wpf.dll</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Charts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>ActiproSoftware.Text.Addons.Xml.Wpf.dll</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Charts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>ActiproSoftware.Text.LLParser.Wpf.dll</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Charts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>ActiproSoftware.Views.Wpf.dll</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>views</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>ActiproSoftware.Wizard.Wpf.dll</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>wizard</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>AgileObjects.NetStandardPolyfills.dll</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Charts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>AgileObjects.ReadableExpressions.dll</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Charts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>AuthenticodeExaminer.dll</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Charts</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>